<commit_message>
Manual Testing notes as on jun24th
</commit_message>
<xml_diff>
--- a/Test Case Template.xlsx
+++ b/Test Case Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\010LiveTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0307E10E-9AD1-49BB-80FA-529C518DE77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349B1EB3-9747-4B3D-B703-FED63B945FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BF258B6-0441-47D3-980D-A0CAF612A56D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Project Name</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>reyaz1212</t>
+  </si>
+  <si>
+    <t>same as expected</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Screenshots</t>
+  </si>
+  <si>
+    <t>D:\010LiveTech\Screenshots\TC001\Screenshot 2024-06-24 100610.png</t>
   </si>
 </sst>
 </file>
@@ -635,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FB5A85-1055-4ACD-81B3-2A5F2F033F25}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -650,13 +662,14 @@
     <col min="6" max="6" width="54.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="93.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="104.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -664,7 +677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -675,7 +688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -683,7 +696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -691,7 +704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -699,7 +712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -733,8 +746,11 @@
       <c r="K6" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="L6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="93.6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -759,11 +775,17 @@
       <c r="H7" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="K7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
@@ -776,8 +798,17 @@
       <c r="H8" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
@@ -790,8 +821,14 @@
       <c r="H9" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
@@ -805,7 +842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
@@ -819,7 +856,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E12" s="1" t="s">
         <v>49</v>
       </c>
@@ -827,7 +864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="93.6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" ht="93.6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -850,7 +887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -864,7 +901,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
@@ -878,7 +915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1042,6 +1079,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L8" r:id="rId1" xr:uid="{74E749C0-C3B2-49C9-AE78-C299B1E24E0F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>